<commit_message>
updated code with all hackathons
</commit_message>
<xml_diff>
--- a/non_contacts.xlsx
+++ b/non_contacts.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://unstop.com/hackathon/hackholyoke-mount-holyoke-481051</t>
+          <t>https://unstop.com/hackathon/queen-city-hacks-queen-city-hacks-490822</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -460,7 +460,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://unstop.com/hackathon/athena-hacks-showcode-480926</t>
+          <t>https://unstop.com/hackathon/rock-hacks-rock-hacks-490603</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -472,7 +472,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://unstop.com/hackathon/rock-hacks-hack-club-479990</t>
+          <t>https://unstop.com/hackathon/hackholyoke-mount-holyoke-481051</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -484,7 +484,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://unstop.com/hackathon/unihacks-unihacks-480103</t>
+          <t>https://unstop.com/hackathon/athena-hacks-showcode-480926</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -496,7 +496,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://unstop.com/hackathon/niural-hackathon-niural-479609</t>
+          <t>https://unstop.com/hackathon/unihacks-unihacks-480103</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -508,7 +508,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://unstop.com/hackathon/hatch-taronga-accelerator-program-2023-taronga-479605</t>
+          <t>https://unstop.com/hackathon/rock-hacks-hack-club-479990</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -520,10 +520,1298 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>https://unstop.com/hackathon/niural-hackathon-niural-479609</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/hatch-taronga-accelerator-program-2023-taronga-479605</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>https://unstop.com/hackathon/spacehack-2022-canberra-innovation-network-cbrin-457878</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/hackmca-middlesex-county-academy-edison-new-jersey-457875</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/xr-hacks-xr-hacks-447994</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/lion-city-hacks-lion-city-hacks-447998</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/quote-to-code-i-pandoras-box-indus-os-439223</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/uga-hacks-university-of-georgia-439175</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/ycp-hacks-york-college-of-pennsylvania-438753</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/hinterland-hack-2022-founders-foundation-433048</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/newhacks-2022-university-of-toronto-436543</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/hackprinceton-princeton-university-436507</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/hackphs-princeton-high-school-436529</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/tamu-datathon-texas-am-university-433023</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/hack-tx-university-of-texas-at-austin-432936</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/unite-hacks-unitehacks-432922</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/plutohacks-broward-college-florida-usa-432942</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/google-code-jam-google-10587</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/kick-start-google-431734</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/lunarhacks-lunar-hacks-430025</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/mhacks-14-university-of-michigan-428530</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/the-pitt-challenge-university-of-pittsburgh-428533</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/ibc-hack-1-ibc-media-im-bangalore-421685</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/hack-austin-coder-one-417616</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/conuhacks-vii-concordia-university-montreal-quebec-420464</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/divhacks-2022-green-screen-columbia-university-new-york-420925</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/kent-hack-enough-kent-hack-enough-419286</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/cal-hacks-university-of-california-berkeley-419275</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/hackumbc-university-of-maryland-418846</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/code-likeabosch-hybrid-hackathon-robert-bosch-gmbh-417623</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/junction-x-budapest-2022-craft-hub-417620</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/hacklytics-2023-georgia-institute-of-technology-409928</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/hack-wash-u-anheuser-busch-409905</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/sachacks-iv-university-of-california-davis-409896</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/medhacks-johns-hopkins-university-408337</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/hack-harvard-harvard-university-cambridge-408357</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/hack-the-valley-6-university-of-toronto-408368</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/hack-orlando-hack-orlando-407674</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/coder-one-coder-one-407677</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/technica-2022-technica-402793</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/leland-hacks-the-hack-foundation-402764</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/breederdao-hackathon-stack-league-397313</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/hackathon-challenge-2022-institute-of-engineering-and-technologyiet-london-397099</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/make-uc-university-of-cincinnati-384538</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/big-red-hacks-big-red-hacks-384407</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/get-set-hack-risecom-383391</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/sego-lily-hacks-sego-lily-hacks-378612</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/pennapps-xxiii-pennapps-378597</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/hophacks-johns-hopkins-university-378564</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/paradigm-conference-2022-paradigm-374361</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/assemble-hackclub-374329</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/world-youth-coders-hackathon-2022-world-coding-club-366313</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/mix-n-match-elysia-2022-sjb-institute-of-technology-sjbit-bengaluru-357204</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/encode-austin-hackathon-encode-club-ltd-354000</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/schoolhacks-schoolhacks-350702</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/hydra-hacks-hydra-hacks-350707</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/call-for-code-global-challenge-2022-call-for-code-348338</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/encode-x-polygon-hackathon-encode-club-ltd-333540</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/nft-berlin-encode-club-nft-berlin-333309</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/encode-x-blocksplit-hackathon-encode-club-ltd-331461</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/code4good-viva-technology-327567</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/sogeti-green-x-game-jam-sogeti-324308</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/high-tech-hacks-20-high-tech-hacks-323712</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/gryph-hacks-university-of-guelph-323739</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/montyhacks-v-montgomery-high-school-322847</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/plasma-hackathon-jawaharlal-nehru-national-college-of-engineering-jnnce-shimoga-karnataka-319483</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/high-tech-hacks-20-high-tech-high-school-secaucus-291005</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/masseyhacks-viii-vincent-massey-secondary-school-canada-290970</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/ru-hacks-2022-ryerson-university-285723</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/code-character-bytehoc-pragyan-seshasayee-institute-of-technologysit-tiruchirappalli-268488</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr"/>
+      <c r="B78" t="inlineStr"/>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/smart-home-sensors-and-analytics-hackathon-resideo-smart-home-technologies-india-private-limited-252321</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/lowes-india-hiring-codeathon-lowes-services-india-pvt-ltd-252329</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/ibm-z-student-contest-ibm-252320</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/source-code-kascade-bihar-jharkhand-kshitij-indian-institute-of-technology-iit-kharagpur-251724</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/cuhackit-2022-college-of-engineering-computing-applied-sciences-clemson-university-251578</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/designathon-build-exun-2021-22-delhi-public-school-r-k-puram-251138</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/source-code-kascade-tamil-nadu-indian-institute-of-technology-iit-kharagpur-251549</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/cruzhacks-2022-university-of-california-santa-cruz-250355</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/kent-hack-enough-kent-hack-enough-246083</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/babylon-project-v2-world-blockchain-hackathon-164223</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/plutohacks-broward-college-florida-usa-224274</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/the-pitt-challenge-university-of-pittsburgh-222296</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/api-hacks-20-api-hacks-216736</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/sunhacks-arizona-state-university-205999</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/shellhacks-florida-international-university-fiu-205200</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/metis-hackathon-metis-203811</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/medhacks-johns-hopkins-university-195355</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/hackrice-11-rice-university-194514</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/datathon-shooting-stars-foundation-192807</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/tamu-datathon-texas-am-university-191959</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/hacks-for-humanity-arizona-state-university-191580</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/sci2change-hackathon-sci2-foundation-190723</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/first-annual-california-artificial-intelligence-summit-girls-computing-league-189824</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/abilityhacks-ablifynow-189082</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/kuriushacks-kurius-188182</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/creatica-2021-creatica-187768</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/healthmetrics-x-imu-hackathon-2021-healthmetrics-186961</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/techacks-20-techacks-185407</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/coastalhacks-coastalhacks-185187</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/gui-development-hackathon-csir-central-mechanical-engineering-research-institute-183607</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/blockathon21-thadomal-shahani-engineering-college-tsec-mumbai-182811</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/orf-unleash-hacks-india-observer-research-foundation-180901</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/pridehacks-major-league-hacking-175276</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/researchathon-researchathon-175076</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/synaptic-hacks-2021-simply-neuroscience-173535</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/hack-the-gap-girlsexe-172858</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/creartathon-inria-170366</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>https://unstop.com/hackathon/mergexindia-hackpolicy-foundation-169176</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
         <is>
           <t>[]</t>
         </is>

</xml_diff>